<commit_message>
pushing beginning of project 2
</commit_message>
<xml_diff>
--- a/Project2/Traduction avis clients/avis_1_traduit.xlsx
+++ b/Project2/Traduction avis clients/avis_1_traduit.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/santiago_martin_edu_devinci_fr/Documents/A5/S1/ML NLP/NLP_Project/Project2/Traduction avis clients/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_962B802BBDFA0BBDC941F8441FE2412509BA81A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_962B802BBDFA0BBDC941F8441FE2412509BA81A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E573BBB8-D408-4329-98C4-810C2E00DA61}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1001</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -9617,9 +9620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -41993,6 +41994,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1001" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>